<commit_message>
dadndo ip a cisco
</commit_message>
<xml_diff>
--- a/CeladitaGaspar_RTxAC_TC7.xlsx
+++ b/CeladitaGaspar_RTxAC_TC7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unmsmmail-my.sharepoint.com/personal/fernando_celadita_unmsm_edu_pe/Documents/Documents-UNMSM/UNMSM/ciclo VI/Redes, Trasnmision y automatizacion y control/sesion7/TC7 NAT y HSRP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="474" documentId="8_{C3A7DD5C-5F27-4C87-8602-6207A2C2178E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB6B5BF0-E373-4896-98F7-1EE183DCFE1A}"/>
+  <xr:revisionPtr revIDLastSave="528" documentId="8_{C3A7DD5C-5F27-4C87-8602-6207A2C2178E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FC91CA5-FD5C-4A28-B77A-7BB146B0B60B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="750">
   <si>
     <t>Router 1</t>
   </si>
@@ -1998,12 +1998,6 @@
     <t>172.16.156.0</t>
   </si>
   <si>
-    <t>172.16.156.00 000000 /26</t>
-  </si>
-  <si>
-    <t>172.16.156.0-255</t>
-  </si>
-  <si>
     <t>172.16.156.255</t>
   </si>
   <si>
@@ -2019,207 +2013,27 @@
     <t>172.16.156.1</t>
   </si>
   <si>
-    <t>azul</t>
-  </si>
-  <si>
-    <t>172.16.156.10 000000 /26</t>
-  </si>
-  <si>
-    <t>172.16.156.11 000000 /26</t>
-  </si>
-  <si>
-    <t>172.16.156.127</t>
-  </si>
-  <si>
-    <t>172.16.156.191</t>
-  </si>
-  <si>
     <t>172.16.156.2</t>
   </si>
   <si>
-    <t>172.16.156.63</t>
-  </si>
-  <si>
-    <t>172.16.156.62</t>
-  </si>
-  <si>
-    <t>172.16.156.126</t>
-  </si>
-  <si>
-    <t>172.16.156.190</t>
-  </si>
-  <si>
     <t>172.16.156.64</t>
   </si>
   <si>
-    <t>172.16.156.0-63</t>
-  </si>
-  <si>
-    <t>172.16.156.64-127</t>
-  </si>
-  <si>
-    <t>172.16.156.192-255</t>
-  </si>
-  <si>
-    <t>172.16.156.128-191</t>
-  </si>
-  <si>
     <t>172.16.156.65</t>
   </si>
   <si>
-    <t>172.16.156.129</t>
-  </si>
-  <si>
-    <t>172.16.156.193</t>
-  </si>
-  <si>
-    <t>172.16.156.010 00000 /27</t>
-  </si>
-  <si>
-    <t>amarillo</t>
-  </si>
-  <si>
     <t>255.255.255.224</t>
   </si>
   <si>
-    <t>172.16.156.95</t>
-  </si>
-  <si>
-    <t>172.16.156.011000 00 /30</t>
-  </si>
-  <si>
-    <t>172.16.156.011001 00 /30</t>
-  </si>
-  <si>
-    <t>172.16.156.96-99</t>
-  </si>
-  <si>
-    <t>172.16.156.100-103</t>
-  </si>
-  <si>
-    <t>172.16.156.99</t>
-  </si>
-  <si>
-    <t>172.16.156.103</t>
-  </si>
-  <si>
     <t>172.16.156.97</t>
   </si>
   <si>
     <t>172.16.156.98</t>
   </si>
   <si>
-    <t>172.16.156.101</t>
-  </si>
-  <si>
-    <t>172.16.156.102</t>
-  </si>
-  <si>
-    <t>172.16.156.011010 00 /30</t>
-  </si>
-  <si>
-    <t>172.16.156.011011 00 /30</t>
-  </si>
-  <si>
-    <t>172.16.156.011100 00 /30</t>
-  </si>
-  <si>
-    <t>172.16.156.011101 00 /30</t>
-  </si>
-  <si>
-    <t>172.16.156.011110 00 /30</t>
-  </si>
-  <si>
-    <t>172.16.156.011111 00 /30</t>
-  </si>
-  <si>
-    <t>VERDE</t>
-  </si>
-  <si>
-    <t>172.16.156.0 /26</t>
-  </si>
-  <si>
-    <t>172.16.156.64 /26</t>
-  </si>
-  <si>
-    <t>172.16.156.96/27</t>
-  </si>
-  <si>
-    <t>172.16.156.104 - 107</t>
-  </si>
-  <si>
-    <t>172.16.156.108-111</t>
-  </si>
-  <si>
-    <t>172.16.156.112-115</t>
-  </si>
-  <si>
-    <t>172.16.156.116-119</t>
-  </si>
-  <si>
-    <t>172.16.156.120-123</t>
-  </si>
-  <si>
-    <t>172.16.156.94</t>
-  </si>
-  <si>
-    <t>172.16.156.64 - 95</t>
-  </si>
-  <si>
-    <t>172.16.156.96 - 127</t>
-  </si>
-  <si>
-    <t>172.16.156.124-127</t>
-  </si>
-  <si>
     <t>255.255.255.0</t>
   </si>
   <si>
-    <t>172.16.156.107</t>
-  </si>
-  <si>
-    <t>172.16.156.111</t>
-  </si>
-  <si>
-    <t>172.16.156.115</t>
-  </si>
-  <si>
-    <t>172.16.156.119</t>
-  </si>
-  <si>
-    <t>172.16.156.123</t>
-  </si>
-  <si>
-    <t>172.16.156.105</t>
-  </si>
-  <si>
-    <t>172.16.156.109</t>
-  </si>
-  <si>
-    <t>172.16.156.113</t>
-  </si>
-  <si>
-    <t>172.16.156.121</t>
-  </si>
-  <si>
-    <t>172.16.156.1125</t>
-  </si>
-  <si>
-    <t>172.16.156.106</t>
-  </si>
-  <si>
-    <t>172.16.156.110</t>
-  </si>
-  <si>
-    <t>172.16.156.114</t>
-  </si>
-  <si>
-    <t>172.16.156.118</t>
-  </si>
-  <si>
-    <t>172.16.156.122</t>
-  </si>
-  <si>
     <t>ROUTER 4</t>
   </si>
   <si>
@@ -2436,10 +2250,43 @@
     <t>G --&gt;6</t>
   </si>
   <si>
-    <t>172.000 10000.00011000.00000000</t>
-  </si>
-  <si>
-    <t>172.16.24.0 /11</t>
+    <t>172.16.24.0 /24</t>
+  </si>
+  <si>
+    <t>172.16.24.0 - 255</t>
+  </si>
+  <si>
+    <t>172.16.24.1</t>
+  </si>
+  <si>
+    <t>172.16.24.2</t>
+  </si>
+  <si>
+    <t>172.16.24.3</t>
+  </si>
+  <si>
+    <t>205.78.23.0/8.</t>
+  </si>
+  <si>
+    <t>205.78.23.1</t>
+  </si>
+  <si>
+    <t>205.78.23.2</t>
+  </si>
+  <si>
+    <t>205.78.23.3</t>
+  </si>
+  <si>
+    <t>98.54.35.0/8</t>
+  </si>
+  <si>
+    <t>98.54.35.1</t>
+  </si>
+  <si>
+    <t>98.54.35.2</t>
+  </si>
+  <si>
+    <t>255.255.0.0</t>
   </si>
 </sst>
 </file>
@@ -2476,7 +2323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2495,20 +2342,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -2724,11 +2559,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2761,9 +2605,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2812,6 +2653,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3257,10 +3107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B060E0A-2540-4047-B4C1-D793BD14044C}">
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3294,7 +3144,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>798</v>
+        <v>736</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>648</v>
@@ -3305,7 +3155,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>797</v>
+        <v>735</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>649</v>
@@ -3322,179 +3172,182 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>799</v>
+        <v>737</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="44" t="s">
         <v>647</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="44" t="s">
         <v>643</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="44" t="s">
         <v>642</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="44" t="s">
         <v>646</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="44" t="s">
         <v>644</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="44" t="s">
         <v>645</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44" t="s">
+        <v>737</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>738</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>664</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>653</v>
+      </c>
+      <c r="G8" s="46" t="s">
+        <v>657</v>
+      </c>
+      <c r="H8" s="46" t="s">
         <v>656</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="D8" s="22" t="s">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>644</v>
+      </c>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44" t="s">
+        <v>739</v>
+      </c>
+      <c r="D11" s="44"/>
+      <c r="E11" s="51" t="s">
+        <v>664</v>
+      </c>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44" t="s">
+        <v>740</v>
+      </c>
+      <c r="D12" s="44"/>
+      <c r="E12" s="51" t="s">
+        <v>664</v>
+      </c>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44" t="s">
+        <v>741</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="E13" s="51" t="s">
+        <v>664</v>
+      </c>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>647</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>643</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>642</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>646</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>644</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>645</v>
+      </c>
+      <c r="G15" s="52" t="s">
         <v>654</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>711</v>
-      </c>
-      <c r="F8" s="22" t="s">
+      <c r="H15" s="52" t="s">
         <v>655</v>
       </c>
-      <c r="G8" s="22" t="s">
-        <v>659</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>643</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>642</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>646</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>644</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>645</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="B12" s="22">
-        <v>38</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>653</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>671</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>666</v>
-      </c>
-      <c r="G12" s="22" t="s">
-        <v>659</v>
-      </c>
-      <c r="H12" s="22" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23" t="s">
-        <v>700</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>672</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>663</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>675</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>674</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>664</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4" t="s">
-        <v>662</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>673</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>655</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>677</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>658</v>
-      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44" t="s">
+        <v>742</v>
+      </c>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44" t="s">
+        <v>749</v>
+      </c>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
+      <c r="B17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -3512,1507 +3365,1459 @@
       <c r="E18" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44" t="s">
+        <v>743</v>
+      </c>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44" t="s">
+        <v>749</v>
+      </c>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44" t="s">
+        <v>744</v>
+      </c>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44" t="s">
+        <v>749</v>
+      </c>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44" t="s">
+        <v>745</v>
+      </c>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44" t="s">
+        <v>749</v>
+      </c>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="47"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+    </row>
+    <row r="23" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
+        <v>647</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>643</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>642</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>646</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>644</v>
+      </c>
+      <c r="F23" s="44" t="s">
         <v>645</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
-        <v>679</v>
-      </c>
-      <c r="B19" s="23">
-        <v>19</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>678</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>708</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>680</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>681</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>675</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24" t="s">
-        <v>701</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>709</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>680</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>663</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>688</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="G23" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="H23" s="44" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44" t="s">
+        <v>749</v>
+      </c>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="45"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>647</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>645</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
-        <v>698</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24" t="s">
-        <v>682</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>684</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="F24" s="24" t="s">
-        <v>686</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>688</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4" t="s">
-        <v>683</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>685</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>687</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>690</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
-        <v>692</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>702</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>712</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>717</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>722</v>
-      </c>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4" t="s">
-        <v>693</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>703</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>718</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>723</v>
-      </c>
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44" t="s">
+        <v>747</v>
+      </c>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44" t="s">
+        <v>749</v>
+      </c>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
-        <v>694</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>704</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>714</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>719</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>724</v>
-      </c>
+      <c r="A28" s="44"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44" t="s">
+        <v>748</v>
+      </c>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44" t="s">
+        <v>749</v>
+      </c>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4" t="s">
-        <v>695</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>705</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>715</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>714</v>
-      </c>
-      <c r="H29" s="4" t="s">
+      <c r="A29" s="47"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="47"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="47"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="47"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="47"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4" t="s">
-        <v>696</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>706</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>716</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>720</v>
-      </c>
-      <c r="H30" s="4" t="s">
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
+      <c r="H36" s="29" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4" t="s">
-        <v>697</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>710</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>663</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>721</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
-        <v>787</v>
-      </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="35"/>
-      <c r="H33" s="32" t="s">
-        <v>788</v>
-      </c>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-    </row>
-    <row r="34" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="B34" s="27" t="s">
-        <v>796</v>
-      </c>
-      <c r="C34" s="25" t="s">
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+    </row>
+    <row r="37" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>733</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>734</v>
+      </c>
+      <c r="C37" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D37" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="E37" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="26" t="s">
+      <c r="F37" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H34" s="30" t="s">
-        <v>795</v>
-      </c>
-      <c r="I34" s="26" t="s">
-        <v>796</v>
-      </c>
-      <c r="J34" s="25" t="s">
+      <c r="H37" s="27" t="s">
+        <v>733</v>
+      </c>
+      <c r="I37" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="J37" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K34" s="26" t="s">
+      <c r="K37" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L34" s="26" t="s">
+      <c r="L37" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="M34" s="26" t="s">
+      <c r="M37" s="23" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>1</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>652</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>727</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="H35" s="4">
-        <v>1</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>670</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>728</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>675</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>680</v>
-      </c>
-      <c r="M35" s="4"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>2</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>652</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>729</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>665</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="H36" s="4">
-        <v>2</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>670</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>768</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>680</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>3</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>652</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>731</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="H37" s="4">
-        <v>3</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>670</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>769</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>680</v>
-      </c>
-      <c r="M37" s="4" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>12</v>
+        <v>665</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>732</v>
+        <v>657</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="4"/>
+      <c r="H38" s="4">
+        <v>1</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H38" s="4">
-        <v>4</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J38" s="4" t="s">
-        <v>63</v>
+        <v>666</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>770</v>
+        <v>660</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>680</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>675</v>
-      </c>
+        <v>661</v>
+      </c>
+      <c r="M38" s="4"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>13</v>
+        <v>667</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>733</v>
+        <v>658</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F39" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H39" s="4">
+        <v>2</v>
+      </c>
+      <c r="I39" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H39" s="4">
-        <v>5</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J39" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>771</v>
+        <v>706</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>734</v>
+        <v>669</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F40" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H40" s="4">
+        <v>3</v>
+      </c>
+      <c r="I40" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H40" s="4">
-        <v>6</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J40" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>772</v>
+        <v>707</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>735</v>
+        <v>670</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F41" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H41" s="4">
+        <v>4</v>
+      </c>
+      <c r="I41" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H41" s="4">
-        <v>7</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J41" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>773</v>
+        <v>708</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>736</v>
+        <v>671</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F42" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H42" s="4">
+        <v>5</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H42" s="4">
-        <v>8</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J42" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>774</v>
+        <v>709</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>737</v>
+        <v>672</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F43" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H43" s="4">
+        <v>6</v>
+      </c>
+      <c r="I43" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H43" s="4">
-        <v>9</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J43" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>775</v>
+        <v>710</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>738</v>
+        <v>673</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F44" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H44" s="4">
+        <v>7</v>
+      </c>
+      <c r="I44" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H44" s="4">
-        <v>10</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J44" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>776</v>
+        <v>711</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>739</v>
+        <v>674</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F45" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H45" s="4">
+        <v>8</v>
+      </c>
+      <c r="I45" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H45" s="4">
-        <v>11</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J45" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>777</v>
+        <v>712</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>740</v>
+        <v>675</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F46" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H46" s="4">
+        <v>9</v>
+      </c>
+      <c r="I46" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="G46" s="31"/>
-      <c r="H46" s="4">
-        <v>12</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J46" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>778</v>
+        <v>713</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>741</v>
+        <v>676</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F47" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H47" s="4">
+        <v>10</v>
+      </c>
+      <c r="I47" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H47" s="4">
-        <v>13</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J47" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>779</v>
+        <v>714</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>742</v>
+        <v>677</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F48" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H48" s="4">
+        <v>11</v>
+      </c>
+      <c r="I48" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H48" s="4">
-        <v>14</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J48" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>780</v>
+        <v>715</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>743</v>
+        <v>678</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F49" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="G49" s="28"/>
+      <c r="H49" s="4">
+        <v>12</v>
+      </c>
+      <c r="I49" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H49" s="4">
-        <v>15</v>
-      </c>
-      <c r="I49" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J49" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>781</v>
+        <v>716</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>744</v>
+        <v>679</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F50" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H50" s="4">
+        <v>13</v>
+      </c>
+      <c r="I50" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H50" s="4">
-        <v>16</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J50" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>782</v>
+        <v>717</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>745</v>
+        <v>680</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F51" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H51" s="4">
+        <v>14</v>
+      </c>
+      <c r="I51" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H51" s="4">
-        <v>17</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J51" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>783</v>
+        <v>718</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>746</v>
+        <v>681</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F52" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H52" s="4">
+        <v>15</v>
+      </c>
+      <c r="I52" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H52" s="4">
-        <v>18</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J52" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>784</v>
+        <v>719</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>747</v>
+        <v>682</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F53" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H53" s="4">
+        <v>16</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H53" s="4">
-        <v>19</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J53" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>785</v>
+        <v>720</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>748</v>
+        <v>683</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F54" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H54" s="4">
+        <v>17</v>
+      </c>
+      <c r="I54" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H54" s="4">
-        <v>20</v>
-      </c>
-      <c r="I54" s="4" t="s">
-        <v>670</v>
-      </c>
       <c r="J54" s="4" t="s">
-        <v>767</v>
+        <v>76</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>786</v>
+        <v>721</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>749</v>
+        <v>684</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F55" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H55" s="4">
+        <v>18</v>
+      </c>
+      <c r="I55" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
+      <c r="J55" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>750</v>
+        <v>685</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F56" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H56" s="4">
+        <v>19</v>
+      </c>
+      <c r="I56" s="4" t="s">
         <v>659</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>751</v>
+        <v>686</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F57" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H57" s="4">
+        <v>20</v>
+      </c>
+      <c r="I57" s="4" t="s">
         <v>659</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>752</v>
+        <v>687</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>730</v>
+        <v>58</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>753</v>
+        <v>688</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>754</v>
+        <v>689</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="I60" s="25" t="s">
-        <v>789</v>
-      </c>
-      <c r="J60" s="26" t="s">
-        <v>790</v>
-      </c>
-      <c r="K60" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="L60" s="26" t="s">
-        <v>9</v>
+        <v>657</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>755</v>
+        <v>690</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="I61" s="28" t="s">
-        <v>793</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>791</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="L61" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>32</v>
+        <v>668</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>756</v>
+        <v>691</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="I62" s="29"/>
-      <c r="J62" s="4" t="s">
-        <v>792</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>688</v>
-      </c>
-      <c r="L62" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>757</v>
+        <v>692</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="I63" s="28" t="s">
-        <v>794</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>791</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>675</v>
-      </c>
-      <c r="L63" s="4" t="s">
-        <v>680</v>
+        <v>657</v>
+      </c>
+      <c r="I63" s="22" t="s">
+        <v>727</v>
+      </c>
+      <c r="J63" s="23" t="s">
+        <v>728</v>
+      </c>
+      <c r="K63" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L63" s="23" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>758</v>
+        <v>693</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="I64" s="29"/>
+        <v>657</v>
+      </c>
+      <c r="I64" s="25" t="s">
+        <v>731</v>
+      </c>
       <c r="J64" s="4" t="s">
-        <v>792</v>
+        <v>729</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>689</v>
+        <v>657</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>759</v>
+        <v>694</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+      <c r="I65" s="26"/>
+      <c r="J65" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="K65" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="L65" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>760</v>
+        <v>695</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+      <c r="I66" s="25" t="s">
+        <v>732</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="K66" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="L66" s="4" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>761</v>
+        <v>696</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+      <c r="I67" s="26"/>
+      <c r="J67" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="L67" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>762</v>
+        <v>697</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>763</v>
+        <v>698</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>764</v>
+        <v>699</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>765</v>
+        <v>700</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>652</v>
       </c>
       <c r="C72" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>36</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>37</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>38</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D72" s="4" t="s">
-        <v>766</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>659</v>
+      <c r="D75" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>657</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="A36:F36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5078,16 +4883,16 @@
         <v>285</v>
       </c>
       <c r="R1" s="10"/>
-      <c r="S1" s="41" t="s">
+      <c r="S1" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="T1" s="42"/>
+      <c r="T1" s="39"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="35" t="s">
         <v>275</v>
       </c>
-      <c r="H2" s="38"/>
+      <c r="H2" s="35"/>
       <c r="N2" s="12" t="s">
         <v>281</v>
       </c>
@@ -5099,10 +4904,10 @@
         <v>285</v>
       </c>
       <c r="R2" s="13"/>
-      <c r="S2" s="43" t="s">
+      <c r="S2" s="40" t="s">
         <v>289</v>
       </c>
-      <c r="T2" s="44"/>
+      <c r="T2" s="41"/>
     </row>
     <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -5111,16 +4916,16 @@
       <c r="N3" t="s">
         <v>282</v>
       </c>
-      <c r="S3" s="45" t="s">
+      <c r="S3" s="42" t="s">
         <v>288</v>
       </c>
-      <c r="T3" s="46"/>
+      <c r="T3" s="43"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="34" t="s">
         <v>602</v>
       </c>
-      <c r="B4" s="37"/>
+      <c r="B4" s="34"/>
       <c r="C4" t="s">
         <v>268</v>
       </c>
@@ -5137,16 +4942,16 @@
       <c r="N4" t="s">
         <v>283</v>
       </c>
-      <c r="S4" s="43" t="s">
+      <c r="S4" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="T4" s="44"/>
+      <c r="T4" s="41"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="34" t="s">
         <v>603</v>
       </c>
-      <c r="B5" s="37"/>
+      <c r="B5" s="34"/>
       <c r="C5" t="s">
         <v>269</v>
       </c>
@@ -5162,25 +4967,25 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="34" t="s">
         <v>604</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="34"/>
       <c r="C6" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="T8" s="37"/>
-      <c r="U8" s="37"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="34"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
@@ -5441,25 +5246,25 @@
     <row r="19" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="33" t="s">
         <v>258</v>
       </c>
-      <c r="E21" s="36"/>
+      <c r="E21" s="33"/>
       <c r="F21" s="6"/>
-      <c r="J21" s="36" t="s">
+      <c r="J21" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="K21" s="36"/>
+      <c r="K21" s="33"/>
       <c r="L21" s="6"/>
-      <c r="P21" s="36" t="s">
+      <c r="P21" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="Q21" s="36"/>
+      <c r="Q21" s="33"/>
       <c r="R21" s="6"/>
-      <c r="V21" s="36" t="s">
+      <c r="V21" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="W21" s="36"/>
+      <c r="W21" s="33"/>
       <c r="X21" s="6"/>
     </row>
     <row r="22" spans="2:30" ht="15.75" x14ac:dyDescent="0.25">
@@ -5527,36 +5332,36 @@
       </c>
     </row>
     <row r="25" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="I25" s="39" t="s">
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="I25" s="36" t="s">
         <v>262</v>
       </c>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="O25" s="40" t="s">
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="O25" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="40"/>
-      <c r="U25" s="40" t="s">
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="U25" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="V25" s="40"/>
-      <c r="W25" s="40"/>
-      <c r="X25" s="40"/>
-      <c r="AA25" s="40" t="s">
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="37"/>
+      <c r="AA25" s="37" t="s">
         <v>264</v>
       </c>
-      <c r="AB25" s="40"/>
-      <c r="AC25" s="40"/>
-      <c r="AD25" s="40"/>
+      <c r="AB25" s="37"/>
+      <c r="AC25" s="37"/>
+      <c r="AD25" s="37"/>
     </row>
     <row r="26" spans="2:30" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">

</xml_diff>